<commit_message>
models_results highlited the best values
</commit_message>
<xml_diff>
--- a/models/models_result.xlsx
+++ b/models/models_result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15740" windowHeight="13260"/>
+    <workbookView windowWidth="17860" windowHeight="13260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Модуль упругости при растяжении</t>
   </si>
@@ -58,13 +58,7 @@
     <t>Lasso_norm</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>DecisionTreeRegressor</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>DecisionTreeRegressor_best</t>
@@ -96,11 +90,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -137,6 +131,120 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -145,60 +253,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -206,72 +260,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -288,49 +282,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,133 +444,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,17 +563,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -608,39 +611,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -648,6 +618,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -666,147 +651,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -816,7 +810,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -855,9 +849,6 @@
     <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -895,14 +886,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1234,8 +1217,8 @@
   <sheetPr/>
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1266,23 +1249,23 @@
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="22" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1303,11 +1286,11 @@
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="22" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="5" t="s">
@@ -1345,26 +1328,26 @@
       <c r="F3" s="7">
         <v>2.1325</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="19">
         <v>2.4773</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="24">
+      <c r="H3" s="20"/>
+      <c r="I3" s="14">
         <v>141389.7205</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="14">
         <v>224732.5402</v>
       </c>
-      <c r="K3" s="24">
+      <c r="K3" s="14">
         <v>0.2756</v>
       </c>
-      <c r="L3" s="24">
+      <c r="L3" s="14">
         <v>0.0013</v>
       </c>
-      <c r="M3" s="24">
+      <c r="M3" s="14">
         <v>300.0945</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="14">
         <v>384.482</v>
       </c>
     </row>
@@ -1390,23 +1373,23 @@
       <c r="G4" s="9">
         <v>2.4501</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="24">
+      <c r="H4" s="20"/>
+      <c r="I4" s="14">
         <v>150521.6349</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="14">
         <v>226238.0916</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="14">
         <v>0.2288</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="14">
         <v>-0.0054</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="14">
         <v>305.7443</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="14">
         <v>384.2891</v>
       </c>
     </row>
@@ -1432,23 +1415,23 @@
       <c r="G5" s="9">
         <v>0.1588</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="24">
+      <c r="H5" s="20"/>
+      <c r="I5" s="14">
         <v>0.0061</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="14">
         <v>0.0403</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="14">
         <v>0.8226</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="14">
         <v>-0.0193</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="14">
         <v>0.0623</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="14">
         <v>0.1625</v>
       </c>
     </row>
@@ -1460,13 +1443,13 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
     </row>
     <row r="7" ht="18" customHeight="1" spans="1:14">
       <c r="A7" s="6" t="s">
@@ -1490,23 +1473,23 @@
       <c r="G7" s="9">
         <v>2.4471</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="24">
+      <c r="H7" s="20"/>
+      <c r="I7" s="14">
         <v>191764.4221</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="14">
         <v>224528.2006</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="14">
         <v>0.0175</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="14">
         <v>0.0022</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="14">
         <v>348.1372</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="14">
         <v>384.1102</v>
       </c>
     </row>
@@ -1532,23 +1515,23 @@
       <c r="G8" s="9">
         <v>2.4543</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="24">
+      <c r="H8" s="20"/>
+      <c r="I8" s="14">
         <v>191887.4816</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="14">
         <v>223679.5537</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="14">
         <v>0.0169</v>
       </c>
-      <c r="L8" s="24">
+      <c r="L8" s="14">
         <v>0.006</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="14">
         <v>348.3619</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="14">
         <v>383.0815</v>
       </c>
     </row>
@@ -1562,7 +1545,7 @@
       <c r="C9" s="9">
         <v>0.0383</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="9">
         <v>0</v>
       </c>
       <c r="E9" s="9">
@@ -1574,23 +1557,23 @@
       <c r="G9" s="9">
         <v>0.1591</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="24">
+      <c r="H9" s="20"/>
+      <c r="I9" s="14">
         <v>0.0343</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="14">
         <v>0.0395</v>
       </c>
-      <c r="K9" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="24">
+      <c r="K9" s="14">
+        <v>0</v>
+      </c>
+      <c r="L9" s="14">
         <v>-26.9966</v>
       </c>
-      <c r="M9" s="24">
+      <c r="M9" s="14">
         <v>0.1469</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="14">
         <v>0.1607</v>
       </c>
     </row>
@@ -1602,59 +1585,59 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
     </row>
     <row r="11" ht="18" customHeight="1" spans="1:14">
       <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="12">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9">
         <v>0</v>
       </c>
       <c r="C11" s="9">
         <v>18.7589</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="9">
         <v>1</v>
       </c>
       <c r="E11" s="9">
         <v>-1.0667</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="9">
         <v>0</v>
       </c>
       <c r="G11" s="9">
         <v>3.5058</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="24">
+      <c r="H11" s="20"/>
+      <c r="I11" s="14">
+        <v>0</v>
+      </c>
+      <c r="J11" s="14">
         <v>412531.9984</v>
       </c>
-      <c r="K11" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="24">
+      <c r="K11" s="14">
+        <v>1</v>
+      </c>
+      <c r="L11" s="14">
         <v>-0.8332</v>
       </c>
-      <c r="M11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="N11" s="24">
+      <c r="M11" s="14">
+        <v>0</v>
+      </c>
+      <c r="N11" s="14">
         <v>505.6368</v>
       </c>
     </row>
     <row r="12" ht="18" customHeight="1" spans="1:14">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="9">
         <v>8.6243</v>
@@ -1674,29 +1657,29 @@
       <c r="G12" s="9">
         <v>2.5229</v>
       </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="24">
+      <c r="H12" s="20"/>
+      <c r="I12" s="14">
         <v>184036.1737</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="14">
         <v>229794.833</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K12" s="14">
         <v>0.0571</v>
       </c>
-      <c r="L12" s="24">
+      <c r="L12" s="14">
         <v>-0.0212</v>
       </c>
-      <c r="M12" s="24">
+      <c r="M12" s="14">
         <v>332.8734</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="14">
         <v>386.5286</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:14">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="9">
         <v>0.0363</v>
@@ -1716,23 +1699,23 @@
       <c r="G13" s="9">
         <v>0.1637</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="24">
+      <c r="H13" s="20"/>
+      <c r="I13" s="14">
         <v>0.0323</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="14">
         <v>0.0403</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="14">
         <v>0.0571</v>
       </c>
-      <c r="L13" s="24">
+      <c r="L13" s="14">
         <v>-0.0212</v>
       </c>
-      <c r="M13" s="24">
+      <c r="M13" s="14">
         <v>0.1395</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="14">
         <v>0.162</v>
       </c>
     </row>
@@ -1744,17 +1727,17 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:14">
       <c r="A15" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="9">
         <v>9.0767</v>
@@ -1774,29 +1757,29 @@
       <c r="G15" s="9">
         <v>2.4806</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="24">
+      <c r="H15" s="20"/>
+      <c r="I15" s="14">
         <v>190223.9471</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15" s="14">
         <v>225364.1789</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="14">
         <v>0.0254</v>
       </c>
-      <c r="L15" s="24">
+      <c r="L15" s="14">
         <v>-0.0015</v>
       </c>
-      <c r="M15" s="24">
+      <c r="M15" s="14">
         <v>346.2832</v>
       </c>
-      <c r="N15" s="24">
+      <c r="N15" s="14">
         <v>385.7366</v>
       </c>
     </row>
     <row r="16" ht="18" customHeight="1" spans="1:14">
       <c r="A16" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="9">
         <v>0.0385</v>
@@ -1816,23 +1799,23 @@
       <c r="G16" s="9">
         <v>0.1591</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="24">
+      <c r="H16" s="20"/>
+      <c r="I16" s="14">
         <v>0.0326</v>
       </c>
-      <c r="J16" s="24">
+      <c r="J16" s="14">
         <v>0.0406</v>
       </c>
-      <c r="K16" s="24">
+      <c r="K16" s="14">
         <v>0.0488</v>
       </c>
-      <c r="L16" s="24">
+      <c r="L16" s="14">
         <v>-0.0276</v>
       </c>
-      <c r="M16" s="24">
+      <c r="M16" s="14">
         <v>0.1435</v>
       </c>
-      <c r="N16" s="24">
+      <c r="N16" s="14">
         <v>0.1636</v>
       </c>
     </row>
@@ -1844,17 +1827,17 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:14">
       <c r="A18" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="9">
         <v>16.476</v>
@@ -1874,165 +1857,165 @@
       <c r="G18" s="9">
         <v>3.2256</v>
       </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="24">
+      <c r="H18" s="20"/>
+      <c r="I18" s="14">
         <v>216378.0788</v>
       </c>
-      <c r="J18" s="24">
+      <c r="J18" s="14">
         <v>263885.3112</v>
       </c>
-      <c r="K18" s="24">
+      <c r="K18" s="14">
         <v>-0.1086</v>
       </c>
-      <c r="L18" s="24">
+      <c r="L18" s="14">
         <v>-0.1727</v>
       </c>
-      <c r="M18" s="24">
+      <c r="M18" s="14">
         <v>368.6177</v>
       </c>
-      <c r="N18" s="24">
+      <c r="N18" s="14">
         <v>417.0691</v>
       </c>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:14">
       <c r="A19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="13">
+        <v>20</v>
+      </c>
+      <c r="B19" s="12">
         <v>0.0387</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="12">
         <v>0.0383</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="12">
         <v>-0.0002</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <v>-0.0019</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <v>0.1588</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="12">
         <v>0.1591</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="16">
+      <c r="H19" s="20"/>
+      <c r="I19" s="15">
         <v>0.0344</v>
       </c>
-      <c r="J19" s="16">
+      <c r="J19" s="15">
         <v>0.0396</v>
       </c>
-      <c r="K19" s="16">
+      <c r="K19" s="15">
         <v>-0.0031</v>
       </c>
-      <c r="L19" s="16">
+      <c r="L19" s="15">
         <v>-0.0013</v>
       </c>
-      <c r="M19" s="16">
+      <c r="M19" s="15">
         <v>0.1473</v>
       </c>
-      <c r="N19" s="16">
+      <c r="N19" s="15">
         <v>0.1611</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:14">
       <c r="A20" s="10"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:14">
       <c r="A21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="15">
+        <v>21</v>
+      </c>
+      <c r="B21" s="14">
         <v>9.0739</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <v>9.044</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="14">
         <v>0.0116</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <v>0.0036</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="14">
         <v>2.4419</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="14">
         <v>2.449</v>
       </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="24">
+      <c r="H21" s="20"/>
+      <c r="I21" s="14">
         <v>191839.198</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J21" s="14">
         <v>223790.0397</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="14">
         <v>0.0172</v>
       </c>
-      <c r="L21" s="24">
+      <c r="L21" s="14">
         <v>0.0055</v>
       </c>
-      <c r="M21" s="24">
+      <c r="M21" s="14">
         <v>348.3967</v>
       </c>
-      <c r="N21" s="24">
+      <c r="N21" s="14">
         <v>383.4161</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="1" spans="1:14">
       <c r="A22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="16">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15">
         <v>0.0382</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="15">
         <v>0.0382</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="15">
         <v>0.0116</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="15">
         <v>0.0011</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="15">
         <v>0.1582</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="15">
         <v>0.1593</v>
       </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="16">
+      <c r="H22" s="20"/>
+      <c r="I22" s="15">
         <v>0.0338</v>
       </c>
-      <c r="J22" s="16">
+      <c r="J22" s="15">
         <v>0.0394</v>
       </c>
-      <c r="K22" s="16">
+      <c r="K22" s="15">
         <v>0.0136</v>
       </c>
-      <c r="L22" s="16">
+      <c r="L22" s="15">
         <v>0.0026</v>
       </c>
-      <c r="M22" s="16">
+      <c r="M22" s="15">
         <v>0.146</v>
       </c>
-      <c r="N22" s="16">
+      <c r="N22" s="15">
         <v>0.1608</v>
       </c>
     </row>
@@ -2041,10 +2024,40 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B22">
-    <cfRule type="top10" dxfId="0" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="12" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C22">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="11" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D22">
+    <cfRule type="top10" dxfId="0" priority="10" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E22">
+    <cfRule type="top10" dxfId="0" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F22">
+    <cfRule type="top10" dxfId="0" priority="8" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G22">
+    <cfRule type="top10" dxfId="0" priority="7" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I22">
+    <cfRule type="top10" dxfId="0" priority="6" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J22">
+    <cfRule type="top10" dxfId="0" priority="5" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K22">
+    <cfRule type="top10" dxfId="0" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L22">
+    <cfRule type="top10" dxfId="0" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M22">
+    <cfRule type="top10" dxfId="0" priority="2" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N22">
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>